<commit_message>
best liear for this phase
</commit_message>
<xml_diff>
--- a/feature_analysis.xlsx
+++ b/feature_analysis.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="155">
   <si>
     <t>Intercept</t>
   </si>
@@ -464,16 +465,40 @@
   </si>
   <si>
     <t>Integer</t>
+  </si>
+  <si>
+    <t>IR2</t>
+  </si>
+  <si>
+    <t>IR3</t>
+  </si>
+  <si>
+    <t>Mod</t>
+  </si>
+  <si>
+    <t>Sev</t>
+  </si>
+  <si>
+    <t>Fa</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>BLQ</t>
+  </si>
+  <si>
+    <t>LwQ</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,12 +540,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -560,7 +579,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -574,14 +593,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
@@ -2524,20 +2536,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -2548,946 +2559,1546 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="8">
-        <v>0.41571433200000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="8">
-        <v>0.3716778</v>
-      </c>
-      <c r="E4" s="7">
-        <f>D4-D3</f>
-        <v>-4.4036532000000017E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="8">
-        <v>0.37270500000000001</v>
-      </c>
-      <c r="E5" s="7">
-        <f t="shared" ref="E5:E68" si="0">D5-D4</f>
-        <v>1.0272000000000059E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="8">
-        <v>0.35852620000000002</v>
-      </c>
-      <c r="E6" s="7">
-        <f t="shared" si="0"/>
-        <v>-1.4178799999999991E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="E7" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.35852620000000002</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.37430780000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="7">
-        <v>0.35385149999999999</v>
-      </c>
-      <c r="E8" s="7">
-        <f>D6-D8</f>
-        <v>4.6747000000000316E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="E9" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.35385149999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="E10" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7">
-        <v>0.35389609999999999</v>
-      </c>
-      <c r="E11" s="7">
-        <f t="shared" si="0"/>
-        <v>0.35389609999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="E12" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.35389609999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7">
-        <v>0.35335830000000001</v>
-      </c>
-      <c r="E13" s="7">
-        <f>D13-D11</f>
-        <v>-5.3779999999997719E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7">
-        <v>0.27663840000000001</v>
-      </c>
-      <c r="E14" s="7">
-        <f t="shared" si="0"/>
-        <v>-7.6719900000000008E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="E15" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.27663840000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="E16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7">
-        <v>0.26130170000000003</v>
-      </c>
-      <c r="E17" s="7">
-        <f>D17-D14</f>
-        <v>-1.5336699999999981E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7">
-        <v>0.26072859999999998</v>
-      </c>
-      <c r="E18" s="7">
-        <f t="shared" si="0"/>
-        <v>-5.7310000000004857E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7">
-        <v>0.2337467</v>
-      </c>
-      <c r="E19" s="7">
-        <f t="shared" si="0"/>
-        <v>-2.6981899999999975E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="E20" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.2337467</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="E21" s="7">
-        <f>D22-D20</f>
-        <v>0.2295005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7">
-        <v>0.2295005</v>
-      </c>
-      <c r="E22" s="7">
-        <f>D22-D19</f>
-        <v>-4.2462000000000055E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="E23" s="7" t="e">
-        <f>D23-#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="E24" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7">
-        <v>0.2254313</v>
-      </c>
-      <c r="E25" s="7">
-        <f>D25-D22</f>
-        <v>-4.069199999999995E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="E26" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.2254313</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7">
-        <v>0.21921109999999999</v>
-      </c>
-      <c r="E27" s="7">
-        <f>D27-D25</f>
-        <v>-6.2202000000000091E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7">
-        <v>0.2179441</v>
-      </c>
-      <c r="E28" s="7">
-        <f t="shared" si="0"/>
-        <v>-1.2669999999999904E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7">
-        <v>0.20757249999999999</v>
-      </c>
-      <c r="E29" s="7">
-        <f t="shared" si="0"/>
-        <v>-1.0371600000000009E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="E30" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.20757249999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="E31" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7">
-        <v>0.20273540000000001</v>
-      </c>
-      <c r="E32" s="7">
-        <f>D32-D29</f>
-        <v>-4.8370999999999831E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="E33" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.20273540000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="E34" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7">
-        <v>0.19903670000000001</v>
-      </c>
-      <c r="E35" s="7">
-        <f>D35-D32</f>
-        <v>-3.6986999999999992E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="E36" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.19903670000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7">
-        <v>0.19845779999999999</v>
-      </c>
-      <c r="E37" s="7">
-        <f>D37-D35</f>
-        <v>-5.7890000000002106E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7">
-        <v>0.1982651</v>
-      </c>
-      <c r="E38" s="7">
-        <f t="shared" si="0"/>
-        <v>-1.926999999999901E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7">
-        <v>0.19756860000000001</v>
-      </c>
-      <c r="E39" s="7">
-        <f t="shared" si="0"/>
-        <v>-6.9649999999998879E-4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="E40" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.19756860000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="7">
-        <v>0.19748840000000001</v>
-      </c>
-      <c r="E41" s="7">
-        <f t="shared" si="0"/>
-        <v>0.19748840000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7">
-        <v>0.1955962</v>
-      </c>
-      <c r="E42" s="7">
-        <f t="shared" si="0"/>
-        <v>-1.8922000000000105E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="E43" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.1955962</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="E44" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="E45" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="7">
-        <v>0.1915181</v>
-      </c>
-      <c r="E46" s="7">
-        <f>D46-D42</f>
-        <v>-4.0781000000000012E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7">
-        <v>0.18992100000000001</v>
-      </c>
-      <c r="E47" s="7">
-        <f t="shared" si="0"/>
-        <v>-1.5970999999999902E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="7">
-        <v>0.1873097</v>
-      </c>
-      <c r="E48" s="7">
-        <f t="shared" si="0"/>
-        <v>-2.6113000000000108E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="E49" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.1873097</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="E50" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="7">
-        <v>0.1847982</v>
-      </c>
-      <c r="E51" s="7">
-        <f>D51-D48</f>
-        <v>-2.5114999999999998E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C51" s="5"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="E52" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.1847982</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="7">
-        <v>0.17967150000000001</v>
-      </c>
-      <c r="E53" s="7">
-        <f>D53-D51</f>
-        <v>-5.126699999999984E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="E54" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.17967150000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="7">
-        <v>0.1763315</v>
-      </c>
-      <c r="E55" s="7">
-        <f t="shared" si="0"/>
-        <v>0.1763315</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C55" s="5"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="7">
-        <v>0.1760737</v>
-      </c>
-      <c r="E56" s="7">
-        <f t="shared" si="0"/>
-        <v>-2.5780000000000247E-4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C56" s="5"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="E57" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.1760737</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="7">
-        <v>0.1746123</v>
-      </c>
-      <c r="E58" s="7">
-        <f>D58-D56</f>
-        <v>-1.4614000000000016E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C58" s="5"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="E59" s="7"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7">
-        <v>0.17168230000000001</v>
-      </c>
-      <c r="E60" s="7">
-        <f>D60-D58</f>
-        <v>-2.9299999999999882E-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="7">
-        <v>0.17150979999999999</v>
-      </c>
-      <c r="E61" s="7">
-        <f t="shared" si="0"/>
-        <v>-1.7250000000001986E-4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="7">
-        <v>0.1710583</v>
-      </c>
-      <c r="E62" s="7">
-        <f t="shared" si="0"/>
-        <v>-4.5149999999999357E-4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C62" s="5"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="E63" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.1710583</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="7">
-        <v>0.16955909999999999</v>
-      </c>
-      <c r="E64" s="7">
-        <f>D64-D62</f>
-        <v>-1.4992000000000061E-3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C64" s="5"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="9"/>
-      <c r="E65" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="E66" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="7">
-        <v>0.16914899999999999</v>
-      </c>
-      <c r="E67" s="7">
-        <f>D67-D64</f>
-        <v>-4.1009999999999658E-4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C67" s="5"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="7">
-        <v>0.1685315</v>
-      </c>
-      <c r="E68" s="7">
-        <f t="shared" si="0"/>
-        <v>-6.1749999999999305E-4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C68" s="5"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="7">
-        <v>0.16798469999999999</v>
-      </c>
-      <c r="E69" s="7">
-        <f t="shared" ref="E69:E83" si="1">D69-D68</f>
-        <v>-5.4680000000001394E-4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C69" s="5"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="9"/>
-      <c r="E70" s="7">
-        <f t="shared" si="1"/>
-        <v>-0.16798469999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="7">
-        <v>0.16776279999999999</v>
-      </c>
-      <c r="E71" s="7">
-        <f t="shared" si="1"/>
-        <v>0.16776279999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C71" s="5"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="7">
-        <v>0.16593330000000001</v>
-      </c>
-      <c r="E72" s="7">
-        <f t="shared" si="1"/>
-        <v>-1.8294999999999839E-3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C72" s="5"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="9"/>
-      <c r="E73" s="7">
-        <f t="shared" si="1"/>
-        <v>-0.16593330000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="9"/>
-      <c r="E74" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="9"/>
-      <c r="E75" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="9"/>
-      <c r="E76" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C76" s="6"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="9"/>
-      <c r="E77" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-      <c r="C78" s="9"/>
-      <c r="E78" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C78" s="6"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="7">
-        <v>0.1655411</v>
-      </c>
-      <c r="E79" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1655411</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C79" s="5"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="7">
-        <v>0.16527890000000001</v>
-      </c>
-      <c r="E80" s="7">
-        <f t="shared" si="1"/>
-        <v>-2.6219999999999022E-4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C80" s="5"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="9"/>
-      <c r="E81" s="7">
-        <f t="shared" si="1"/>
-        <v>-0.16527890000000001</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C81" s="6"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-      <c r="E82" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
-      </c>
-      <c r="E83" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I119"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" t="str">
+        <f>A1&amp;" = ifelse("&amp;A1&amp;" == '"&amp;B1&amp;"', 5, ifelse("&amp;A1&amp;" == '"&amp;C1&amp;"', 4, ifelse("&amp;A1&amp;" == '"&amp;D1&amp;"',  3, ifelse("&amp;A1&amp;" == '"&amp;E1&amp;"', 2, ifelse('"&amp;A1&amp;" == "&amp;F1&amp;"', 1, 0)))))"</f>
+        <v>ExterQual = ifelse(ExterQual == 'Ex', 5, ifelse(ExterQual == 'Gd', 4, ifelse(ExterQual == 'TA',  3, ifelse(ExterQual == 'Fa', 2, ifelse('ExterQual == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I17" si="0">A2&amp;" = ifelse("&amp;A2&amp;" == '"&amp;B2&amp;"', 5, ifelse("&amp;A2&amp;" == '"&amp;C2&amp;"', 4, ifelse("&amp;A2&amp;" == '"&amp;D2&amp;"',  3, ifelse("&amp;A2&amp;" == '"&amp;E2&amp;"', 2, ifelse('"&amp;A2&amp;" == "&amp;F2&amp;"', 1, 0)))))"</f>
+        <v>ExterCond = ifelse(ExterCond == 'Ex', 5, ifelse(ExterCond == 'Gd', 4, ifelse(ExterCond == 'TA',  3, ifelse(ExterCond == 'Fa', 2, ifelse('ExterCond == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v>BsmtQual = ifelse(BsmtQual == 'Ex', 5, ifelse(BsmtQual == 'Gd', 4, ifelse(BsmtQual == 'TA',  3, ifelse(BsmtQual == 'Fa', 2, ifelse('BsmtQual == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>BsmtCond = ifelse(BsmtCond == 'Ex', 5, ifelse(BsmtCond == 'Gd', 4, ifelse(BsmtCond == 'TA',  3, ifelse(BsmtCond == 'Fa', 2, ifelse('BsmtCond == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>HeatingQC = ifelse(HeatingQC == 'Ex', 5, ifelse(HeatingQC == 'Gd', 4, ifelse(HeatingQC == 'TA',  3, ifelse(HeatingQC == 'Fa', 2, ifelse('HeatingQC == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>KitchenQual = ifelse(KitchenQual == 'Ex', 5, ifelse(KitchenQual == 'Gd', 4, ifelse(KitchenQual == 'TA',  3, ifelse(KitchenQual == 'Fa', 2, ifelse('KitchenQual == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>FireplaceQu = ifelse(FireplaceQu == 'Ex', 5, ifelse(FireplaceQu == 'Gd', 4, ifelse(FireplaceQu == 'TA',  3, ifelse(FireplaceQu == 'Fa', 2, ifelse('FireplaceQu == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>GarageQual = ifelse(GarageQual == 'Ex', 5, ifelse(GarageQual == 'Gd', 4, ifelse(GarageQual == 'TA',  3, ifelse(GarageQual == 'Fa', 2, ifelse('GarageQual == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>GarageCond = ifelse(GarageCond == 'Ex', 5, ifelse(GarageCond == 'Gd', 4, ifelse(GarageCond == 'TA',  3, ifelse(GarageCond == 'Fa', 2, ifelse('GarageCond == Po', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>PoolQC = ifelse(PoolQC == 'Ex', 5, ifelse(PoolQC == 'Gd', 4, ifelse(PoolQC == 'TA',  3, ifelse(PoolQC == 'Fa', 2, ifelse('PoolQC == No', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>GarageFinish = ifelse(GarageFinish == 'Fin', 5, ifelse(GarageFinish == 'RFn', 4, ifelse(GarageFinish == 'Unf',  3, ifelse(GarageFinish == 'No', 2, ifelse('GarageFinish == ', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>BsmtExposure = ifelse(BsmtExposure == 'Gd', 5, ifelse(BsmtExposure == 'Av', 4, ifelse(BsmtExposure == 'Mn',  3, ifelse(BsmtExposure == 'No', 2, ifelse('BsmtExposure == ', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>BsmtFinType1 = ifelse(BsmtFinType1 == 'GLQ', 5, ifelse(BsmtFinType1 == 'ALQ', 4, ifelse(BsmtFinType1 == 'BLQ',  3, ifelse(BsmtFinType1 == 'Rec', 2, ifelse('BsmtFinType1 == LwQ', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>BsmtFinType2 = ifelse(BsmtFinType2 == 'GLQ', 5, ifelse(BsmtFinType2 == 'ALQ', 4, ifelse(BsmtFinType2 == 'BLQ',  3, ifelse(BsmtFinType2 == 'Rec', 2, ifelse('BsmtFinType2 == LwQ', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" t="s">
+        <v>149</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>LandSlope = ifelse(LandSlope == 'Gtl', 5, ifelse(LandSlope == 'Mod', 4, ifelse(LandSlope == 'Sev',  3, ifelse(LandSlope == '', 2, ifelse('LandSlope == ', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>CentralAir = ifelse(CentralAir == 'N', 5, ifelse(CentralAir == 'Y', 4, ifelse(CentralAir == '',  3, ifelse(CentralAir == '', 2, ifelse('CentralAir == ', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>LotShape = ifelse(LotShape == 'Reg', 5, ifelse(LotShape == 'IR1', 4, ifelse(LotShape == 'IR2',  3, ifelse(LotShape == 'IR3', 2, ifelse('LotShape == ', 1, 0)))))</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I18" t="str">
+        <f>"total$"&amp;A1&amp;" = as.numeric(total$"&amp;A1&amp;")"</f>
+        <v>total$ExterQual = as.numeric(total$ExterQual)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I19" t="str">
+        <f t="shared" ref="I19:I82" si="1">"total$"&amp;A2&amp;" = as.numeric(total$"&amp;A2&amp;")"</f>
+        <v>total$ExterCond = as.numeric(total$ExterCond)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>total$BsmtQual = as.numeric(total$BsmtQual)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>total$BsmtCond = as.numeric(total$BsmtCond)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>total$HeatingQC = as.numeric(total$HeatingQC)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v>total$KitchenQual = as.numeric(total$KitchenQual)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v>total$FireplaceQu = as.numeric(total$FireplaceQu)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v>total$GarageQual = as.numeric(total$GarageQual)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v>total$GarageCond = as.numeric(total$GarageCond)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v>total$PoolQC = as.numeric(total$PoolQC)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I28" t="str">
+        <f t="shared" si="1"/>
+        <v>total$GarageFinish = as.numeric(total$GarageFinish)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I29" t="str">
+        <f t="shared" si="1"/>
+        <v>total$BsmtExposure = as.numeric(total$BsmtExposure)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I30" t="str">
+        <f t="shared" si="1"/>
+        <v>total$BsmtFinType1 = as.numeric(total$BsmtFinType1)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I31" t="str">
+        <f t="shared" si="1"/>
+        <v>total$BsmtFinType2 = as.numeric(total$BsmtFinType2)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I32" t="str">
+        <f t="shared" si="1"/>
+        <v>total$LandSlope = as.numeric(total$LandSlope)</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" t="str">
+        <f t="shared" si="1"/>
+        <v>total$CentralAir = as.numeric(total$CentralAir)</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I34" t="str">
+        <f t="shared" si="1"/>
+        <v>total$LotShape = as.numeric(total$LotShape)</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I35" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I36" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I37" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I38" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I39" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I40" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I41" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I42" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I43" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I44" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I45" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I46" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I48" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I53" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I54" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I55" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I56" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I57" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I58" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I59" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I60" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I61" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I62" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I63" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I64" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I65" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I66" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I67" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I68" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I69" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I70" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I71" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I72" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I73" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I74" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I75" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I76" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I77" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I78" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I79" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I80" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I81" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I82" t="str">
+        <f t="shared" si="1"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I83" t="str">
+        <f t="shared" ref="I83:I119" si="2">"total$"&amp;A66&amp;" = as.numeric(total$"&amp;A66&amp;")"</f>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I84" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I85" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I86" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I87" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I88" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I89" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I90" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I91" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I92" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I93" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I94" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I95" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I96" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I97" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I98" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I99" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I100" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I101" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I102" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I103" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I104" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I105" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I106" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I107" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I108" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I109" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I110" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="111" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I111" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="112" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I112" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="113" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I113" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="114" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I114" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="115" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I115" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="116" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I116" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="117" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I117" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="118" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I118" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+    <row r="119" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I119" t="str">
+        <f t="shared" si="2"/>
+        <v>total$ = as.numeric(total$)</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:H17">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>